<commit_message>
Update Release 1 - Estimates.xlsx
</commit_message>
<xml_diff>
--- a/Release 1 - Estimates.xlsx
+++ b/Release 1 - Estimates.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deshuklasachithanandam/My Business/Wavilla/Release Activities/Release 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deshuklasachithanandam/Desktop/Venkatesh Internship Tasks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05A886F-63EB-5B48-870F-3383DE29B2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E910AFD-352C-CE4F-8375-3AF9DBD76439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{2B95A81A-FB61-1E47-A781-149137CCC044}"/>
   </bookViews>
   <sheets>
     <sheet name="Work BreakDown" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Work BreakDown'!$A$1:$G$347</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
   <si>
     <t>Module Name</t>
   </si>
@@ -126,6 +129,12 @@
   </si>
   <si>
     <t>Home Page / Feed Page</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>Create, Update, Preview, List, Change Status</t>
   </si>
 </sst>
 </file>
@@ -513,10 +522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D4A203-1C5A-7748-A2E2-A669AB2F24A1}">
-  <dimension ref="A1:F347"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G347"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,9 +535,10 @@
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -546,8 +557,11 @@
       <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -563,8 +577,11 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -581,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -598,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -615,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -635,7 +652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -655,7 +672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -672,7 +689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <f>A8+1</f>
         <v>8</v>
@@ -690,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ref="A10:A73" si="0">A9+1</f>
         <v>9</v>
@@ -708,7 +725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -728,8 +745,11 @@
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -749,8 +769,11 @@
       <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -770,8 +793,11 @@
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -791,8 +817,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -812,8 +841,11 @@
       <c r="F15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -833,8 +865,11 @@
       <c r="F16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -854,8 +889,11 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -875,8 +913,11 @@
       <c r="F18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -896,8 +937,11 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -915,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -933,1963 +977,1975 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" ref="A74:A137" si="1">A73+1</f>
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" si="1"/>
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="1"/>
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" si="1"/>
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" si="1"/>
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136">
         <f t="shared" si="1"/>
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" si="1"/>
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138">
         <f t="shared" ref="A138:A201" si="2">A137+1</f>
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139">
         <f t="shared" si="2"/>
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140">
         <f t="shared" si="2"/>
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142">
         <f t="shared" si="2"/>
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143">
         <f t="shared" si="2"/>
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144">
         <f t="shared" si="2"/>
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145">
         <f t="shared" si="2"/>
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146">
         <f t="shared" si="2"/>
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147">
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148">
         <f t="shared" si="2"/>
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149">
         <f t="shared" si="2"/>
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150">
         <f t="shared" si="2"/>
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152">
         <f t="shared" si="2"/>
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153">
         <f t="shared" si="2"/>
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154">
         <f t="shared" si="2"/>
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155">
         <f t="shared" si="2"/>
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156">
         <f t="shared" si="2"/>
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157">
         <f t="shared" si="2"/>
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158">
         <f t="shared" si="2"/>
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159">
         <f t="shared" si="2"/>
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160">
         <f t="shared" si="2"/>
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161">
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162">
         <f t="shared" si="2"/>
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163">
         <f t="shared" si="2"/>
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164">
         <f t="shared" si="2"/>
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165">
         <f t="shared" si="2"/>
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166">
         <f t="shared" si="2"/>
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167">
         <f t="shared" si="2"/>
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168">
         <f t="shared" si="2"/>
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169">
         <f t="shared" si="2"/>
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170">
         <f t="shared" si="2"/>
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171">
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172">
         <f t="shared" si="2"/>
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173">
         <f t="shared" si="2"/>
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174">
         <f t="shared" si="2"/>
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175">
         <f t="shared" si="2"/>
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176">
         <f t="shared" si="2"/>
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177">
         <f t="shared" si="2"/>
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178">
         <f t="shared" si="2"/>
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179">
         <f t="shared" si="2"/>
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180">
         <f t="shared" si="2"/>
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182">
         <f t="shared" si="2"/>
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183">
         <f t="shared" si="2"/>
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184">
         <f t="shared" si="2"/>
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185">
         <f t="shared" si="2"/>
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186">
         <f t="shared" si="2"/>
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187">
         <f t="shared" si="2"/>
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188">
         <f t="shared" si="2"/>
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189">
         <f t="shared" si="2"/>
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190">
         <f t="shared" si="2"/>
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191">
         <f t="shared" si="2"/>
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192">
         <f t="shared" si="2"/>
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193">
         <f t="shared" si="2"/>
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194">
         <f t="shared" si="2"/>
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195">
         <f t="shared" si="2"/>
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196">
         <f t="shared" si="2"/>
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197">
         <f t="shared" si="2"/>
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198">
         <f t="shared" si="2"/>
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199">
         <f t="shared" si="2"/>
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200">
         <f t="shared" si="2"/>
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202">
         <f t="shared" ref="A202:A265" si="3">A201+1</f>
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203">
         <f t="shared" si="3"/>
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204">
         <f t="shared" si="3"/>
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205">
         <f t="shared" si="3"/>
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206">
         <f t="shared" si="3"/>
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207">
         <f t="shared" si="3"/>
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208">
         <f t="shared" si="3"/>
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209">
         <f t="shared" si="3"/>
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210">
         <f t="shared" si="3"/>
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211">
         <f t="shared" si="3"/>
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212">
         <f t="shared" si="3"/>
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213">
         <f t="shared" si="3"/>
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214">
         <f t="shared" si="3"/>
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215">
         <f t="shared" si="3"/>
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216">
         <f t="shared" si="3"/>
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217">
         <f t="shared" si="3"/>
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218">
         <f t="shared" si="3"/>
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219">
         <f t="shared" si="3"/>
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220">
         <f t="shared" si="3"/>
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221">
         <f t="shared" si="3"/>
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222">
         <f t="shared" si="3"/>
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223">
         <f t="shared" si="3"/>
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224">
         <f t="shared" si="3"/>
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225">
         <f t="shared" si="3"/>
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226">
         <f t="shared" si="3"/>
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227">
         <f t="shared" si="3"/>
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228">
         <f t="shared" si="3"/>
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229">
         <f t="shared" si="3"/>
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230">
         <f t="shared" si="3"/>
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231">
         <f t="shared" si="3"/>
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232">
         <f t="shared" si="3"/>
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233">
         <f t="shared" si="3"/>
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234">
         <f t="shared" si="3"/>
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235">
         <f t="shared" si="3"/>
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236">
         <f t="shared" si="3"/>
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237">
         <f t="shared" si="3"/>
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238">
         <f t="shared" si="3"/>
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239">
         <f t="shared" si="3"/>
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240">
         <f t="shared" si="3"/>
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241">
         <f t="shared" si="3"/>
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242">
         <f t="shared" si="3"/>
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243">
         <f t="shared" si="3"/>
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244">
         <f t="shared" si="3"/>
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245">
         <f t="shared" si="3"/>
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246">
         <f t="shared" si="3"/>
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247">
         <f t="shared" si="3"/>
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248">
         <f t="shared" si="3"/>
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249">
         <f t="shared" si="3"/>
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250">
         <f t="shared" si="3"/>
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251">
         <f t="shared" si="3"/>
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252">
         <f t="shared" si="3"/>
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253">
         <f t="shared" si="3"/>
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254">
         <f t="shared" si="3"/>
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255">
         <f t="shared" si="3"/>
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256">
         <f t="shared" si="3"/>
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257">
         <f t="shared" si="3"/>
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258">
         <f t="shared" si="3"/>
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259">
         <f t="shared" si="3"/>
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260">
         <f t="shared" si="3"/>
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261">
         <f t="shared" si="3"/>
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262">
         <f t="shared" si="3"/>
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263">
         <f t="shared" si="3"/>
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264">
         <f t="shared" si="3"/>
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265">
         <f t="shared" si="3"/>
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266">
         <f t="shared" ref="A266:A329" si="4">A265+1</f>
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267">
         <f t="shared" si="4"/>
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268">
         <f t="shared" si="4"/>
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269">
         <f t="shared" si="4"/>
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270">
         <f t="shared" si="4"/>
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271">
         <f t="shared" si="4"/>
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272">
         <f t="shared" si="4"/>
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273">
         <f t="shared" si="4"/>
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274">
         <f t="shared" si="4"/>
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275">
         <f t="shared" si="4"/>
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276">
         <f t="shared" si="4"/>
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277">
         <f t="shared" si="4"/>
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278">
         <f t="shared" si="4"/>
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279">
         <f t="shared" si="4"/>
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280">
         <f t="shared" si="4"/>
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281">
         <f t="shared" si="4"/>
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282">
         <f t="shared" si="4"/>
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283">
         <f t="shared" si="4"/>
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284">
         <f t="shared" si="4"/>
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285">
         <f t="shared" si="4"/>
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286">
         <f t="shared" si="4"/>
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287">
         <f t="shared" si="4"/>
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288">
         <f t="shared" si="4"/>
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289">
         <f t="shared" si="4"/>
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290">
         <f t="shared" si="4"/>
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291">
         <f t="shared" si="4"/>
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292">
         <f t="shared" si="4"/>
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293">
         <f t="shared" si="4"/>
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294">
         <f t="shared" si="4"/>
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295">
         <f t="shared" si="4"/>
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296">
         <f t="shared" si="4"/>
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297">
         <f t="shared" si="4"/>
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298">
         <f t="shared" si="4"/>
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299">
         <f t="shared" si="4"/>
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300">
         <f t="shared" si="4"/>
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301">
         <f t="shared" si="4"/>
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302">
         <f t="shared" si="4"/>
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303">
         <f t="shared" si="4"/>
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304">
         <f t="shared" si="4"/>
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305">
         <f t="shared" si="4"/>
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306">
         <f t="shared" si="4"/>
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307">
         <f t="shared" si="4"/>
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308">
         <f t="shared" si="4"/>
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309">
         <f t="shared" si="4"/>
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310">
         <f t="shared" si="4"/>
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311">
         <f t="shared" si="4"/>
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312">
         <f t="shared" si="4"/>
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313">
         <f t="shared" si="4"/>
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314">
         <f t="shared" si="4"/>
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315">
         <f t="shared" si="4"/>
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316">
         <f t="shared" si="4"/>
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317">
         <f t="shared" si="4"/>
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318">
         <f t="shared" si="4"/>
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319">
         <f t="shared" si="4"/>
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320">
         <f t="shared" si="4"/>
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321">
         <f t="shared" si="4"/>
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322">
         <f t="shared" si="4"/>
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323">
         <f t="shared" si="4"/>
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324">
         <f t="shared" si="4"/>
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325">
         <f t="shared" si="4"/>
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326">
         <f t="shared" si="4"/>
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327">
         <f t="shared" si="4"/>
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328">
         <f t="shared" si="4"/>
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329">
         <f t="shared" si="4"/>
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330">
         <f t="shared" ref="A330:A347" si="5">A329+1</f>
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331">
         <f t="shared" si="5"/>
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332">
         <f t="shared" si="5"/>
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333">
         <f t="shared" si="5"/>
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334">
         <f t="shared" si="5"/>
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335">
         <f t="shared" si="5"/>
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336">
         <f t="shared" si="5"/>
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337">
         <f t="shared" si="5"/>
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A338">
         <f t="shared" si="5"/>
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339">
         <f t="shared" si="5"/>
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340">
         <f t="shared" si="5"/>
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341">
         <f t="shared" si="5"/>
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342">
         <f t="shared" si="5"/>
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343">
         <f t="shared" si="5"/>
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344">
         <f t="shared" si="5"/>
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345">
         <f t="shared" si="5"/>
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346">
         <f t="shared" si="5"/>
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347">
         <f t="shared" si="5"/>
         <v>346</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G347" xr:uid="{04D4A203-1C5A-7748-A2E2-A669AB2F24A1}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Admin Portal"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Jira stories task completed
</commit_message>
<xml_diff>
--- a/Release 1 - Estimates.xlsx
+++ b/Release 1 - Estimates.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deshuklasachithanandam/Desktop/Venkatesh Internship Tasks/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC8A6CD-1E48-E44F-8C4D-A4C388005186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{2B95A81A-FB61-1E47-A781-149137CCC044}"/>
+    <workbookView windowWidth="12708" windowHeight="8112"/>
   </bookViews>
   <sheets>
     <sheet name="Work BreakDown" sheetId="1" r:id="rId1"/>
@@ -20,9 +14,6 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -41,13 +32,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
   <si>
+    <t>Sno</t>
+  </si>
+  <si>
     <t>Module Name</t>
   </si>
   <si>
-    <t>Sno</t>
-  </si>
-  <si>
-    <t>App Language Setup</t>
+    <t>Linked To Item</t>
   </si>
   <si>
     <t>App Type</t>
@@ -56,7 +47,22 @@
     <t>Role</t>
   </si>
   <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>App Language Setup</t>
+  </si>
+  <si>
     <t>Admin Portal</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Create, Update, Preview, List, Change Status</t>
   </si>
   <si>
     <t>Select Language</t>
@@ -77,10 +83,7 @@
     <t>Manage Operator List</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Release</t>
+    <t>Manage Contract Type</t>
   </si>
   <si>
     <t>Account Setup</t>
@@ -93,12 +96,6 @@
   </si>
   <si>
     <t>Manage Gender</t>
-  </si>
-  <si>
-    <t>Manage Contract Type</t>
-  </si>
-  <si>
-    <t>Linked To Item</t>
   </si>
   <si>
     <t>Manage Job Role</t>
@@ -130,30 +127,23 @@
   <si>
     <t>Home Page / Feed Page</t>
   </si>
-  <si>
-    <t>Actions</t>
-  </si>
-  <si>
-    <t>Create, Update, Preview, List, Change Status</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -161,18 +151,363 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -180,26 +515,312 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -248,7 +869,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -281,26 +902,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -333,23 +937,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -511,2429 +1098,2427 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D4A203-1C5A-7748-A2E2-A669AB2F24A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G347"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="11.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="10.1666666666667" customWidth="1"/>
+    <col min="7" max="7" width="37.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <f>A8+1</f>
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10">
         <f t="shared" ref="A10:A73" si="0">A9+1</f>
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C14">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C15">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C17">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1">
       <c r="A71">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1">
       <c r="A72">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1">
       <c r="A73">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1">
       <c r="A74">
         <f t="shared" ref="A74:A137" si="1">A73+1</f>
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1">
       <c r="A101">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1">
       <c r="A102">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1">
       <c r="A103">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1">
       <c r="A104">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1">
       <c r="A105">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1">
       <c r="A106">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1">
       <c r="A107">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1">
       <c r="A108">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1">
       <c r="A109">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1">
       <c r="A110">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1">
       <c r="A111">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1">
       <c r="A112">
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1">
       <c r="A113">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1">
       <c r="A114">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1">
       <c r="A115">
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1">
       <c r="A116">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1">
       <c r="A117">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1">
       <c r="A118">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1">
       <c r="A119">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1">
       <c r="A120">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1">
       <c r="A121">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1">
       <c r="A122">
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1">
       <c r="A123">
         <f t="shared" si="1"/>
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1">
       <c r="A124">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1">
       <c r="A125">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1">
       <c r="A126">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1">
       <c r="A127">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1">
       <c r="A128">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1">
       <c r="A129">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1">
       <c r="A130">
         <f t="shared" si="1"/>
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1">
       <c r="A131">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1">
       <c r="A132">
         <f t="shared" si="1"/>
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1">
       <c r="A133">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1">
       <c r="A134">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1">
       <c r="A135">
         <f t="shared" si="1"/>
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1">
       <c r="A136">
         <f t="shared" si="1"/>
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1">
       <c r="A137">
         <f t="shared" si="1"/>
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1">
       <c r="A138">
         <f t="shared" ref="A138:A201" si="2">A137+1</f>
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1">
       <c r="A139">
         <f t="shared" si="2"/>
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1">
       <c r="A140">
         <f t="shared" si="2"/>
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1">
       <c r="A141">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1">
       <c r="A142">
         <f t="shared" si="2"/>
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1">
       <c r="A143">
         <f t="shared" si="2"/>
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1">
       <c r="A144">
         <f t="shared" si="2"/>
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1">
       <c r="A145">
         <f t="shared" si="2"/>
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1">
       <c r="A146">
         <f t="shared" si="2"/>
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1">
       <c r="A147">
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1">
       <c r="A148">
         <f t="shared" si="2"/>
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1">
       <c r="A149">
         <f t="shared" si="2"/>
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1">
       <c r="A150">
         <f t="shared" si="2"/>
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1">
       <c r="A151">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1">
       <c r="A152">
         <f t="shared" si="2"/>
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1">
       <c r="A153">
         <f t="shared" si="2"/>
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1">
       <c r="A154">
         <f t="shared" si="2"/>
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1">
       <c r="A155">
         <f t="shared" si="2"/>
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1">
       <c r="A156">
         <f t="shared" si="2"/>
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1">
       <c r="A157">
         <f t="shared" si="2"/>
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1">
       <c r="A158">
         <f t="shared" si="2"/>
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1">
       <c r="A159">
         <f t="shared" si="2"/>
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1">
       <c r="A160">
         <f t="shared" si="2"/>
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1">
       <c r="A161">
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1">
       <c r="A162">
         <f t="shared" si="2"/>
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1">
       <c r="A163">
         <f t="shared" si="2"/>
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1">
       <c r="A164">
         <f t="shared" si="2"/>
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1">
       <c r="A165">
         <f t="shared" si="2"/>
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1">
       <c r="A166">
         <f t="shared" si="2"/>
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1">
       <c r="A167">
         <f t="shared" si="2"/>
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1">
       <c r="A168">
         <f t="shared" si="2"/>
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1">
       <c r="A169">
         <f t="shared" si="2"/>
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1">
       <c r="A170">
         <f t="shared" si="2"/>
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1">
       <c r="A171">
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1">
       <c r="A172">
         <f t="shared" si="2"/>
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1">
       <c r="A173">
         <f t="shared" si="2"/>
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1">
       <c r="A174">
         <f t="shared" si="2"/>
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1">
       <c r="A175">
         <f t="shared" si="2"/>
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1">
       <c r="A176">
         <f t="shared" si="2"/>
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1">
       <c r="A177">
         <f t="shared" si="2"/>
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1">
       <c r="A178">
         <f t="shared" si="2"/>
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1">
       <c r="A179">
         <f t="shared" si="2"/>
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1">
       <c r="A180">
         <f t="shared" si="2"/>
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1">
       <c r="A181">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1">
       <c r="A182">
         <f t="shared" si="2"/>
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1">
       <c r="A183">
         <f t="shared" si="2"/>
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1">
       <c r="A184">
         <f t="shared" si="2"/>
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1">
       <c r="A185">
         <f t="shared" si="2"/>
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1">
       <c r="A186">
         <f t="shared" si="2"/>
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1">
       <c r="A187">
         <f t="shared" si="2"/>
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1">
       <c r="A188">
         <f t="shared" si="2"/>
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1">
       <c r="A189">
         <f t="shared" si="2"/>
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1">
       <c r="A190">
         <f t="shared" si="2"/>
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1">
       <c r="A191">
         <f t="shared" si="2"/>
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1">
       <c r="A192">
         <f t="shared" si="2"/>
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1">
       <c r="A193">
         <f t="shared" si="2"/>
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1">
       <c r="A194">
         <f t="shared" si="2"/>
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1">
       <c r="A195">
         <f t="shared" si="2"/>
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1">
       <c r="A196">
         <f t="shared" si="2"/>
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1">
       <c r="A197">
         <f t="shared" si="2"/>
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1">
       <c r="A198">
         <f t="shared" si="2"/>
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1">
       <c r="A199">
         <f t="shared" si="2"/>
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1">
       <c r="A200">
         <f t="shared" si="2"/>
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1">
       <c r="A201">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1">
       <c r="A202">
         <f t="shared" ref="A202:A265" si="3">A201+1</f>
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1">
       <c r="A203">
         <f t="shared" si="3"/>
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1">
       <c r="A204">
         <f t="shared" si="3"/>
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1">
       <c r="A205">
         <f t="shared" si="3"/>
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1">
       <c r="A206">
         <f t="shared" si="3"/>
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1">
       <c r="A207">
         <f t="shared" si="3"/>
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1">
       <c r="A208">
         <f t="shared" si="3"/>
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1">
       <c r="A209">
         <f t="shared" si="3"/>
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1">
       <c r="A210">
         <f t="shared" si="3"/>
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1">
       <c r="A211">
         <f t="shared" si="3"/>
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1">
       <c r="A212">
         <f t="shared" si="3"/>
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1">
       <c r="A213">
         <f t="shared" si="3"/>
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1">
       <c r="A214">
         <f t="shared" si="3"/>
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1">
       <c r="A215">
         <f t="shared" si="3"/>
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:1">
       <c r="A216">
         <f t="shared" si="3"/>
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:1">
       <c r="A217">
         <f t="shared" si="3"/>
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1">
       <c r="A218">
         <f t="shared" si="3"/>
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1">
       <c r="A219">
         <f t="shared" si="3"/>
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1">
       <c r="A220">
         <f t="shared" si="3"/>
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:1">
       <c r="A221">
         <f t="shared" si="3"/>
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:1">
       <c r="A222">
         <f t="shared" si="3"/>
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:1">
       <c r="A223">
         <f t="shared" si="3"/>
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:1">
       <c r="A224">
         <f t="shared" si="3"/>
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:1">
       <c r="A225">
         <f t="shared" si="3"/>
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:1">
       <c r="A226">
         <f t="shared" si="3"/>
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:1">
       <c r="A227">
         <f t="shared" si="3"/>
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:1">
       <c r="A228">
         <f t="shared" si="3"/>
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:1">
       <c r="A229">
         <f t="shared" si="3"/>
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:1">
       <c r="A230">
         <f t="shared" si="3"/>
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:1">
       <c r="A231">
         <f t="shared" si="3"/>
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:1">
       <c r="A232">
         <f t="shared" si="3"/>
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:1">
       <c r="A233">
         <f t="shared" si="3"/>
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:1">
       <c r="A234">
         <f t="shared" si="3"/>
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:1">
       <c r="A235">
         <f t="shared" si="3"/>
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:1">
       <c r="A236">
         <f t="shared" si="3"/>
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:1">
       <c r="A237">
         <f t="shared" si="3"/>
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:1">
       <c r="A238">
         <f t="shared" si="3"/>
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:1">
       <c r="A239">
         <f t="shared" si="3"/>
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:1">
       <c r="A240">
         <f t="shared" si="3"/>
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:1">
       <c r="A241">
         <f t="shared" si="3"/>
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:1">
       <c r="A242">
         <f t="shared" si="3"/>
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:1">
       <c r="A243">
         <f t="shared" si="3"/>
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:1">
       <c r="A244">
         <f t="shared" si="3"/>
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:1">
       <c r="A245">
         <f t="shared" si="3"/>
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:1">
       <c r="A246">
         <f t="shared" si="3"/>
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:1">
       <c r="A247">
         <f t="shared" si="3"/>
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:1">
       <c r="A248">
         <f t="shared" si="3"/>
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:1">
       <c r="A249">
         <f t="shared" si="3"/>
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:1">
       <c r="A250">
         <f t="shared" si="3"/>
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:1">
       <c r="A251">
         <f t="shared" si="3"/>
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:1">
       <c r="A252">
         <f t="shared" si="3"/>
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:1">
       <c r="A253">
         <f t="shared" si="3"/>
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:1">
       <c r="A254">
         <f t="shared" si="3"/>
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:1">
       <c r="A255">
         <f t="shared" si="3"/>
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:1">
       <c r="A256">
         <f t="shared" si="3"/>
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:1">
       <c r="A257">
         <f t="shared" si="3"/>
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:1">
       <c r="A258">
         <f t="shared" si="3"/>
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:1">
       <c r="A259">
         <f t="shared" si="3"/>
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:1">
       <c r="A260">
         <f t="shared" si="3"/>
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:1">
       <c r="A261">
         <f t="shared" si="3"/>
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:1">
       <c r="A262">
         <f t="shared" si="3"/>
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:1">
       <c r="A263">
         <f t="shared" si="3"/>
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:1">
       <c r="A264">
         <f t="shared" si="3"/>
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:1">
       <c r="A265">
         <f t="shared" si="3"/>
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:1">
       <c r="A266">
         <f t="shared" ref="A266:A329" si="4">A265+1</f>
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:1">
       <c r="A267">
         <f t="shared" si="4"/>
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:1">
       <c r="A268">
         <f t="shared" si="4"/>
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:1">
       <c r="A269">
         <f t="shared" si="4"/>
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:1">
       <c r="A270">
         <f t="shared" si="4"/>
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:1">
       <c r="A271">
         <f t="shared" si="4"/>
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:1">
       <c r="A272">
         <f t="shared" si="4"/>
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:1">
       <c r="A273">
         <f t="shared" si="4"/>
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:1">
       <c r="A274">
         <f t="shared" si="4"/>
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:1">
       <c r="A275">
         <f t="shared" si="4"/>
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:1">
       <c r="A276">
         <f t="shared" si="4"/>
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:1">
       <c r="A277">
         <f t="shared" si="4"/>
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:1">
       <c r="A278">
         <f t="shared" si="4"/>
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:1">
       <c r="A279">
         <f t="shared" si="4"/>
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:1">
       <c r="A280">
         <f t="shared" si="4"/>
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:1">
       <c r="A281">
         <f t="shared" si="4"/>
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:1">
       <c r="A282">
         <f t="shared" si="4"/>
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:1">
       <c r="A283">
         <f t="shared" si="4"/>
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:1">
       <c r="A284">
         <f t="shared" si="4"/>
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:1">
       <c r="A285">
         <f t="shared" si="4"/>
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:1">
       <c r="A286">
         <f t="shared" si="4"/>
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:1">
       <c r="A287">
         <f t="shared" si="4"/>
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:1">
       <c r="A288">
         <f t="shared" si="4"/>
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:1">
       <c r="A289">
         <f t="shared" si="4"/>
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:1">
       <c r="A290">
         <f t="shared" si="4"/>
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:1">
       <c r="A291">
         <f t="shared" si="4"/>
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:1">
       <c r="A292">
         <f t="shared" si="4"/>
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:1">
       <c r="A293">
         <f t="shared" si="4"/>
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:1">
       <c r="A294">
         <f t="shared" si="4"/>
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:1">
       <c r="A295">
         <f t="shared" si="4"/>
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:1">
       <c r="A296">
         <f t="shared" si="4"/>
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:1">
       <c r="A297">
         <f t="shared" si="4"/>
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:1">
       <c r="A298">
         <f t="shared" si="4"/>
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:1">
       <c r="A299">
         <f t="shared" si="4"/>
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:1">
       <c r="A300">
         <f t="shared" si="4"/>
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:1">
       <c r="A301">
         <f t="shared" si="4"/>
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:1">
       <c r="A302">
         <f t="shared" si="4"/>
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:1">
       <c r="A303">
         <f t="shared" si="4"/>
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:1">
       <c r="A304">
         <f t="shared" si="4"/>
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:1">
       <c r="A305">
         <f t="shared" si="4"/>
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:1">
       <c r="A306">
         <f t="shared" si="4"/>
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:1">
       <c r="A307">
         <f t="shared" si="4"/>
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:1">
       <c r="A308">
         <f t="shared" si="4"/>
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:1">
       <c r="A309">
         <f t="shared" si="4"/>
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:1">
       <c r="A310">
         <f t="shared" si="4"/>
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:1">
       <c r="A311">
         <f t="shared" si="4"/>
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:1">
       <c r="A312">
         <f t="shared" si="4"/>
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:1">
       <c r="A313">
         <f t="shared" si="4"/>
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:1">
       <c r="A314">
         <f t="shared" si="4"/>
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:1">
       <c r="A315">
         <f t="shared" si="4"/>
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:1">
       <c r="A316">
         <f t="shared" si="4"/>
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:1">
       <c r="A317">
         <f t="shared" si="4"/>
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:1">
       <c r="A318">
         <f t="shared" si="4"/>
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:1">
       <c r="A319">
         <f t="shared" si="4"/>
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:1">
       <c r="A320">
         <f t="shared" si="4"/>
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:1">
       <c r="A321">
         <f t="shared" si="4"/>
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:1">
       <c r="A322">
         <f t="shared" si="4"/>
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:1">
       <c r="A323">
         <f t="shared" si="4"/>
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:1">
       <c r="A324">
         <f t="shared" si="4"/>
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:1">
       <c r="A325">
         <f t="shared" si="4"/>
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:1">
       <c r="A326">
         <f t="shared" si="4"/>
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:1">
       <c r="A327">
         <f t="shared" si="4"/>
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:1">
       <c r="A328">
         <f t="shared" si="4"/>
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:1">
       <c r="A329">
         <f t="shared" si="4"/>
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:1">
       <c r="A330">
         <f t="shared" ref="A330:A347" si="5">A329+1</f>
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:1">
       <c r="A331">
         <f t="shared" si="5"/>
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:1">
       <c r="A332">
         <f t="shared" si="5"/>
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:1">
       <c r="A333">
         <f t="shared" si="5"/>
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:1">
       <c r="A334">
         <f t="shared" si="5"/>
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:1">
       <c r="A335">
         <f t="shared" si="5"/>
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:1">
       <c r="A336">
         <f t="shared" si="5"/>
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:1">
       <c r="A337">
         <f t="shared" si="5"/>
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:1">
       <c r="A338">
         <f t="shared" si="5"/>
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:1">
       <c r="A339">
         <f t="shared" si="5"/>
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:1">
       <c r="A340">
         <f t="shared" si="5"/>
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:1">
       <c r="A341">
         <f t="shared" si="5"/>
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:1">
       <c r="A342">
         <f t="shared" si="5"/>
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:1">
       <c r="A343">
         <f t="shared" si="5"/>
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:1">
       <c r="A344">
         <f t="shared" si="5"/>
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:1">
       <c r="A345">
         <f t="shared" si="5"/>
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:1">
       <c r="A346">
         <f t="shared" si="5"/>
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:1">
       <c r="A347">
         <f t="shared" si="5"/>
         <v>346</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G347" xr:uid="{04D4A203-1C5A-7748-A2E2-A669AB2F24A1}"/>
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G347" etc:filterBottomFollowUsedRange="0">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>